<commit_message>
# Burndown chart para el reporte de avance del 04/10/2010
</commit_message>
<xml_diff>
--- a/meetings/helpers/BurndownChart.20101004.xlsx
+++ b/meetings/helpers/BurndownChart.20101004.xlsx
@@ -1,65 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="270" windowWidth="23295" windowHeight="10680" activeTab="1"/>
+    <workbookView xWindow="840" yWindow="270" windowWidth="19320" windowHeight="10680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
     <sheet name="Burndown Chart" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
-  <si>
-    <t>Crear el mockup de la pagina de las estadisticas globales de un Supervisor para los Jefe de Cuentas y Supervisores (utilizando un dashboard)</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de estadisticas y estado del sueldo variable de un Agente para los Jefes de Cuentas, Supervisores y Agentes (utilizar un dashboard)</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de Login para los usuarios del sistema (Jefes de Cuentas, Supervisores y Agentes)</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de ABM de usuario para el Responsable de IT</t>
-  </si>
-  <si>
-    <t>Crear la estructura inicial de la solucion SelfManagent con todos los proyectos requeridos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>completed</t>
   </si>
   <si>
-    <t>Crear VPC con ambiente de desarrollo</t>
-  </si>
-  <si>
     <t>Puntos</t>
   </si>
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Crear el diseño general de la master page del sistema SelfManagement</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de ABM de Campañas para los Jefes de Cuentas</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de estadisticas globales de las Campañas para los Jefes de Cuentas (utilizando un dashboard y soportando busquedas)</t>
-  </si>
-  <si>
-    <t>Diseñar el esquema de la base de datos para el sistema SelfManagement</t>
-  </si>
-  <si>
-    <t>Implementar la pantalla de alta de campañas para el sistema SelfManagement</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -70,6 +37,51 @@
   </si>
   <si>
     <t>Remaining</t>
+  </si>
+  <si>
+    <t>Modificar el esquema de la base de datos para soportar multiples Supervisores por CampañaEsquemaEsquemaEsquemaEsquemaEsquema</t>
+  </si>
+  <si>
+    <t>Modificar el repositorio que accede a la base de datos para guardar la nueva Campaña</t>
+  </si>
+  <si>
+    <t>Modificar la pantalla de Alta de Campañas para soportar multiples Supervisores</t>
+  </si>
+  <si>
+    <t>Analizar en detalle en que consiste cada una de las metricas a implementar en el sistema SelfManagement</t>
+  </si>
+  <si>
+    <t>Diseñar una interfaz / clase abstracta común para todas las métricas</t>
+  </si>
+  <si>
+    <t>Implementar el repositorio para acceder a la base de datos (lectura y escritura)</t>
+  </si>
+  <si>
+    <t>Implementar la logica del calculo de la parte variable del sueldo en base a las metricas</t>
+  </si>
+  <si>
+    <t>Implementar la logica para proyectar el sueldo variable a fin de mes en base a las tendencias de las metricas</t>
+  </si>
+  <si>
+    <t>Agregar soporte a la pantalla de estadisticas de Agentes para mostrar el sueldo variable calculado y el proyectado</t>
+  </si>
+  <si>
+    <t>Implementar el alta/baja/modificacion de los Agentes en batch desde el archivo de Human Force</t>
+  </si>
+  <si>
+    <t>Implementar la pantalla de estadisticas de Agentes</t>
+  </si>
+  <si>
+    <t>Implementar las métricas seleccionadas para el sistema SelfManagement usando la interfaz comun como base</t>
+  </si>
+  <si>
+    <t>Implementar la logica génerica de procesamiento de las metricas en base a los archivos de los sistemas externos usando la interfaz comun a todas</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -105,16 +117,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,7 +143,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES_tradnl"/>
   <c:style val="11"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -149,52 +169,52 @@
             <c:numRef>
               <c:f>'Burndown Chart'!$A$2:$A$16</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>40434</c:v>
+                  <c:v>40448</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40435</c:v>
+                  <c:v>40449</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40436</c:v>
+                  <c:v>40450</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40437</c:v>
+                  <c:v>40451</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40438</c:v>
+                  <c:v>40452</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40439</c:v>
+                  <c:v>40453</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40440</c:v>
+                  <c:v>40454</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40441</c:v>
+                  <c:v>40455</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40442</c:v>
+                  <c:v>40456</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40443</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40444</c:v>
+                  <c:v>40458</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40445</c:v>
+                  <c:v>40459</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40446</c:v>
+                  <c:v>40460</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40447</c:v>
+                  <c:v>40461</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40448</c:v>
+                  <c:v>40462</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -206,74 +226,60 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="89433600"/>
-        <c:axId val="89435136"/>
+        <c:axId val="92558464"/>
+        <c:axId val="92560000"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="89433600"/>
+        <c:axId val="92558464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89435136"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92560000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="89435136"/>
+        <c:axId val="92560000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -286,7 +292,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="en-US"/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-ES"/>
@@ -300,7 +306,17 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89433600"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92558464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -309,7 +325,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -351,13 +367,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D12" totalsRowShown="0">
-  <autoFilter ref="A1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Title"/>
     <tableColumn id="2" name="Weight"/>
     <tableColumn id="3" name="Status"/>
-    <tableColumn id="4" name="Remaining">
+    <tableColumn id="4" name="Remaining" dataDxfId="0">
       <calculatedColumnFormula>D1-B1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -369,7 +385,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B16" totalsRowShown="0">
   <autoFilter ref="A1:B16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="1" name="Fecha" dataDxfId="1"/>
     <tableColumn id="2" name="Puntos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -661,15 +677,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="145.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="132.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
@@ -677,91 +693,91 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f>SUM(B2:B12)</f>
-        <v>18</v>
+        <f>SUM(B2:B14)</f>
+        <v>19</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f>D2-B2</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D12" si="0">D3-B3</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -770,13 +786,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -785,13 +801,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -800,43 +816,43 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -848,14 +864,44 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ref="D13:D14" si="1">D12-B12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -871,7 +917,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -882,23 +928,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>40434</v>
+        <v>40448</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>40435</v>
+        <v>40449</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -906,15 +952,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>40436</v>
+        <v>40450</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>40437</v>
+        <v>40451</v>
       </c>
       <c r="B5">
         <v>17</v>
@@ -922,90 +968,66 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>40438</v>
+        <v>40452</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>40439</v>
+        <v>40453</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>40440</v>
+        <v>40454</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>40441</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
+        <v>40455</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>40442</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
+        <v>40456</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>40443</v>
-      </c>
-      <c r="B11">
-        <v>14</v>
+        <v>40457</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>40444</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
+        <v>40458</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>40445</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
+        <v>40459</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>40446</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
+        <v>40460</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>40447</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
+        <v>40461</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>40448</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
+        <v>40462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>